<commit_message>
minsafesalary bug fixed (min --> max) + calc_reward positive
</commit_message>
<xml_diff>
--- a/reports/~opt_report.xlsx
+++ b/reports/~opt_report.xlsx
@@ -8,32 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iesegnet-my.sharepoint.com/personal/s_rostami_ieseg_fr/Documents/Research/Papers/2020-eNPV_Contract/NPV Risk Contract - Python/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{85367256-D072-4264-81BD-5F47F57A3562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1688291C-29DC-4DBE-A00E-23A8B13B4B9E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8DF1E4E-2010-40CD-A2D9-0B71AA970FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-3760" windowWidth="38620" windowHeight="21100" xr2:uid="{C6ACAEB0-783C-42D1-903D-11C0FB2671EC}"/>
+    <workbookView xWindow="26340" yWindow="-3650" windowWidth="28700" windowHeight="20880" xr2:uid="{C3295565-4CD6-4476-B445-92EA83605EE5}"/>
   </bookViews>
   <sheets>
     <sheet name="~opt_report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="17">
   <si>
     <t xml:space="preserve">time      </t>
   </si>
@@ -944,11 +931,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{955CA179-9172-46B2-BF2C-E302D541064D}">
-  <dimension ref="A1:N101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069A0938-AD6D-4028-9BA5-3745A98884EC}">
+  <dimension ref="A1:M105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:N5"/>
+      <selection sqref="A1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,10 +950,9 @@
     <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="13" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="76.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1007,9 +993,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>45946.816307870373</v>
+        <v>45947.860277777778</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1047,14 +1033,10 @@
       <c r="M2">
         <v>-23728.748870830001</v>
       </c>
-      <c r="N2" t="str">
-        <f>UPPER(C2)&amp;" &amp; "&amp;ROUND(D2,0)&amp;" &amp; "&amp;TEXT(ROUND(E2, 3), "0.000")&amp;" &amp; "&amp;ROUND(F2,0)&amp;" &amp; "&amp;TEXT(ROUND(I2, 2), "0.00")&amp;" &amp; "&amp;TEXT(ROUND(J2, 2), "0.00")&amp;" &amp; "&amp;TEXT(ROUND(K2, 3), "0.000")&amp;" &amp; "&amp;TEXT(ROUND(L2, 3), "0.000")&amp;" &amp; "&amp;TEXT(ROUND(M2, 3), "0.000")&amp;" \\ "</f>
-        <v xml:space="preserve">LS         &amp; 37261 &amp; 0.000 &amp; 0 &amp; 30.00 &amp; 37.79 &amp; -10440.156 &amp; -13288.593 &amp; -23728.749 \\ </v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>45946.816307870373</v>
+        <v>45947.860277777778</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1092,14 +1074,10 @@
       <c r="M3">
         <v>-19581.01250298</v>
       </c>
-      <c r="N3" t="str">
-        <f t="shared" ref="N3:N5" si="0">UPPER(C3)&amp;" &amp; "&amp;ROUND(D3,0)&amp;" &amp; "&amp;TEXT(ROUND(E3, 3), "0.000")&amp;" &amp; "&amp;ROUND(F3,0)&amp;" &amp; "&amp;TEXT(ROUND(I3, 2), "0.00")&amp;" &amp; "&amp;TEXT(ROUND(J3, 2), "0.00")&amp;" &amp; "&amp;TEXT(ROUND(K3, 3), "0.000")&amp;" &amp; "&amp;TEXT(ROUND(L3, 3), "0.000")&amp;" &amp; "&amp;TEXT(ROUND(M3, 3), "0.000")&amp;" \\ "</f>
-        <v xml:space="preserve">CP         &amp; 17137 &amp; 0.789 &amp; 0 &amp; 0.45 &amp; 38.93 &amp; -4128.288 &amp; -15452.724 &amp; -19581.013 \\ </v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>45946.816307870373</v>
+        <v>45947.860277777778</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1137,14 +1115,10 @@
       <c r="M4">
         <v>-23728.748870830001</v>
       </c>
-      <c r="N4" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">LH         &amp; 37261 &amp; 0.000 &amp; 0 &amp; 30.00 &amp; 37.79 &amp; -10440.156 &amp; -13288.593 &amp; -23728.749 \\ </v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>45946.816307870373</v>
+        <v>45947.860277777778</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1153,13 +1127,13 @@
         <v>16</v>
       </c>
       <c r="D5">
-        <v>9794.0516000000007</v>
+        <v>9794.0375000000004</v>
       </c>
       <c r="E5">
         <v>0.875</v>
       </c>
       <c r="F5">
-        <v>1066.3218999999999</v>
+        <v>1066.3249000000001</v>
       </c>
       <c r="G5">
         <v>5000</v>
@@ -1171,25 +1145,21 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>41.57260084</v>
+        <v>41.572606589999999</v>
       </c>
       <c r="K5">
-        <v>-1945.1945842800001</v>
+        <v>-1945.1897798699999</v>
       </c>
       <c r="L5">
-        <v>-17635.817918699999</v>
+        <v>-17635.82272312</v>
       </c>
       <c r="M5">
         <v>-19581.01250298</v>
       </c>
-      <c r="N5" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">TM         &amp; 9794 &amp; 0.875 &amp; 1066 &amp; 0.00 &amp; 41.57 &amp; -1945.195 &amp; -17635.818 &amp; -19581.013 \\ </v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>45946.816319444442</v>
+        <v>45947.860312500001</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -1228,9 +1198,9 @@
         <v>-25044.314767219999</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>45946.816319444442</v>
+        <v>45947.860312500001</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -1269,9 +1239,9 @@
         <v>-19581.01250298</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>45946.816319444442</v>
+        <v>45947.860312500001</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -1310,9 +1280,9 @@
         <v>-25044.314767219999</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>45946.816319444442</v>
+        <v>45947.860312500001</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -1321,13 +1291,13 @@
         <v>16</v>
       </c>
       <c r="D9">
-        <v>9105.5539000000008</v>
+        <v>6556.9814999999999</v>
       </c>
       <c r="E9">
-        <v>0.90620000000000001</v>
+        <v>0.9375</v>
       </c>
       <c r="F9">
-        <v>406.85730000000001</v>
+        <v>795.09079999999994</v>
       </c>
       <c r="G9">
         <v>5000</v>
@@ -1339,21 +1309,21 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>41.476687640000002</v>
+        <v>42.259746649999997</v>
       </c>
       <c r="K9">
-        <v>-1644.01114904</v>
+        <v>-849.17548319000002</v>
       </c>
       <c r="L9">
-        <v>-17937.001353939999</v>
+        <v>-18731.83701979</v>
       </c>
       <c r="M9">
         <v>-19581.01250298</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>45946.816342592596</v>
+        <v>45947.860335648147</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -1392,9 +1362,9 @@
         <v>-24473.25574651</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>45946.816342592596</v>
+        <v>45947.860335648147</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -1433,9 +1403,9 @@
         <v>-19581.01250298</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>45946.816342592596</v>
+        <v>45947.860335648147</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -1474,9 +1444,9 @@
         <v>-24473.25574651</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>45946.816342592596</v>
+        <v>45947.860335648147</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -1485,13 +1455,13 @@
         <v>16</v>
       </c>
       <c r="D13">
-        <v>10956.6113</v>
+        <v>10956.5903</v>
       </c>
       <c r="E13">
         <v>0.875</v>
       </c>
       <c r="F13">
-        <v>411.50799999999998</v>
+        <v>411.51229999999998</v>
       </c>
       <c r="G13">
         <v>5000</v>
@@ -1503,21 +1473,21 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>40.97894582</v>
+        <v>40.978954770000001</v>
       </c>
       <c r="K13">
-        <v>-2253.73165823</v>
+        <v>-2253.72451477</v>
       </c>
       <c r="L13">
-        <v>-17327.280844739998</v>
+        <v>-17327.287988209999</v>
       </c>
       <c r="M13">
         <v>-19581.01250298</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>45946.816354166665</v>
+        <v>45947.860347222224</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -1556,9 +1526,9 @@
         <v>-23003.34567617</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>45946.816354166665</v>
+        <v>45947.860347222224</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -1597,9 +1567,9 @@
         <v>-19581.01250298</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>45946.816354166665</v>
+        <v>45947.860347222224</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -1640,7 +1610,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>45946.816354166665</v>
+        <v>45947.860347222224</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -1649,13 +1619,13 @@
         <v>16</v>
       </c>
       <c r="D17">
-        <v>19638.249500000002</v>
+        <v>19638.2444</v>
       </c>
       <c r="E17">
         <v>0.75</v>
       </c>
       <c r="F17">
-        <v>168.20869999999999</v>
+        <v>168.2097</v>
       </c>
       <c r="G17">
         <v>5000</v>
@@ -1664,16 +1634,16 @@
         <v>34931.287956369997</v>
       </c>
       <c r="I17">
-        <v>3.8787370000000001</v>
+        <v>3.8787267399999998</v>
       </c>
       <c r="J17">
-        <v>38.234151480000001</v>
+        <v>38.234154539999999</v>
       </c>
       <c r="K17">
-        <v>-4815.9892148400004</v>
+        <v>-4815.9874668499997</v>
       </c>
       <c r="L17">
-        <v>-14765.023288140001</v>
+        <v>-14765.02503613</v>
       </c>
       <c r="M17">
         <v>-19581.01250298</v>
@@ -1681,7 +1651,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>45946.816377314812</v>
+        <v>45947.86037037037</v>
       </c>
       <c r="B18">
         <v>5</v>
@@ -1722,7 +1692,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>45946.816377314812</v>
+        <v>45947.86037037037</v>
       </c>
       <c r="B19">
         <v>5</v>
@@ -1763,7 +1733,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>45946.816377314812</v>
+        <v>45947.86037037037</v>
       </c>
       <c r="B20">
         <v>5</v>
@@ -1804,7 +1774,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>45946.816377314812</v>
+        <v>45947.86037037037</v>
       </c>
       <c r="B21">
         <v>5</v>
@@ -1813,13 +1783,13 @@
         <v>16</v>
       </c>
       <c r="D21">
-        <v>17088.091700000001</v>
+        <v>29032.355599999999</v>
       </c>
       <c r="E21">
-        <v>0.75</v>
+        <v>0.625</v>
       </c>
       <c r="F21">
-        <v>2132.6462999999999</v>
+        <v>579.71770000000004</v>
       </c>
       <c r="G21">
         <v>5000</v>
@@ -1828,16 +1798,16 @@
         <v>27431.287956370001</v>
       </c>
       <c r="I21">
-        <v>0.37637492</v>
+        <v>16.934994240000002</v>
       </c>
       <c r="J21">
-        <v>40.478018749999997</v>
+        <v>35.279112050000002</v>
       </c>
       <c r="K21">
-        <v>-3890.3852566099999</v>
+        <v>-7069.7191078200003</v>
       </c>
       <c r="L21">
-        <v>-15690.627246370001</v>
+        <v>-12511.29339517</v>
       </c>
       <c r="M21">
         <v>-19581.01250298</v>
@@ -1845,7 +1815,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>45946.816388888888</v>
+        <v>45947.860393518517</v>
       </c>
       <c r="B22">
         <v>6</v>
@@ -1886,7 +1856,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>45946.816388888888</v>
+        <v>45947.860393518517</v>
       </c>
       <c r="B23">
         <v>6</v>
@@ -1927,7 +1897,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>45946.816388888888</v>
+        <v>45947.860393518517</v>
       </c>
       <c r="B24">
         <v>6</v>
@@ -1968,7 +1938,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>45946.816388888888</v>
+        <v>45947.860393518517</v>
       </c>
       <c r="B25">
         <v>6</v>
@@ -1977,13 +1947,13 @@
         <v>16</v>
       </c>
       <c r="D25">
-        <v>39626.342100000002</v>
+        <v>39626.280700000003</v>
       </c>
       <c r="E25">
         <v>0.5</v>
       </c>
       <c r="F25">
-        <v>2955.6563999999998</v>
+        <v>2955.6691000000001</v>
       </c>
       <c r="G25">
         <v>5000</v>
@@ -1992,16 +1962,16 @@
         <v>12431.287956370001</v>
       </c>
       <c r="I25">
-        <v>21.025731910000001</v>
+        <v>21.025635359999999</v>
       </c>
       <c r="J25">
-        <v>34.958539729999998</v>
+        <v>34.958602329999998</v>
       </c>
       <c r="K25">
-        <v>-8397.8580844099997</v>
+        <v>-8397.8371097300005</v>
       </c>
       <c r="L25">
-        <v>-11183.15441857</v>
+        <v>-11183.17539325</v>
       </c>
       <c r="M25">
         <v>-19581.01250298</v>
@@ -2009,7 +1979,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>45946.816481481481</v>
+        <v>45947.860509259262</v>
       </c>
       <c r="B26">
         <v>7</v>
@@ -2050,7 +2020,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>45946.816481481481</v>
+        <v>45947.860509259262</v>
       </c>
       <c r="B27">
         <v>7</v>
@@ -2091,7 +2061,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>45946.816481481481</v>
+        <v>45947.860509259262</v>
       </c>
       <c r="B28">
         <v>7</v>
@@ -2132,7 +2102,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>45946.816481481481</v>
+        <v>45947.860509259262</v>
       </c>
       <c r="B29">
         <v>7</v>
@@ -2141,13 +2111,13 @@
         <v>16</v>
       </c>
       <c r="D29">
-        <v>4882.1040000000003</v>
+        <v>4882.1301999999996</v>
       </c>
       <c r="E29">
         <v>0.92279999999999995</v>
       </c>
       <c r="F29">
-        <v>1590.6532999999999</v>
+        <v>1590.652</v>
       </c>
       <c r="G29">
         <v>5000</v>
@@ -2159,21 +2129,21 @@
         <v>0</v>
       </c>
       <c r="J29">
-        <v>43.888429360000003</v>
+        <v>43.888427350000001</v>
       </c>
       <c r="K29">
-        <v>-666.11597169000004</v>
+        <v>-666.11843336000004</v>
       </c>
       <c r="L29">
-        <v>-19364.136958229999</v>
+        <v>-19364.134496549999</v>
       </c>
       <c r="M29">
-        <v>-20030.252929909999</v>
+        <v>-20030.252929900002</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>45946.816504629627</v>
+        <v>45947.860532407409</v>
       </c>
       <c r="B30">
         <v>8</v>
@@ -2214,7 +2184,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>45946.816504629627</v>
+        <v>45947.860532407409</v>
       </c>
       <c r="B31">
         <v>8</v>
@@ -2255,7 +2225,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>45946.816504629627</v>
+        <v>45947.860532407409</v>
       </c>
       <c r="B32">
         <v>8</v>
@@ -2296,7 +2266,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>45946.816504629627</v>
+        <v>45947.860532407409</v>
       </c>
       <c r="B33">
         <v>8</v>
@@ -2305,13 +2275,13 @@
         <v>16</v>
       </c>
       <c r="D33">
-        <v>9046.2587999999996</v>
+        <v>9046.2767999999996</v>
       </c>
       <c r="E33">
         <v>0.875</v>
       </c>
       <c r="F33">
-        <v>962.43010000000004</v>
+        <v>962.42629999999997</v>
       </c>
       <c r="G33">
         <v>5000</v>
@@ -2323,21 +2293,21 @@
         <v>0</v>
       </c>
       <c r="J33">
-        <v>42.331161870000003</v>
+        <v>42.331155080000002</v>
       </c>
       <c r="K33">
-        <v>-1865.03030956</v>
+        <v>-1865.0368653200001</v>
       </c>
       <c r="L33">
-        <v>-17587.131064929999</v>
+        <v>-17587.124509180001</v>
       </c>
       <c r="M33">
-        <v>-19452.161374489999</v>
+        <v>-19452.1613745</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>45946.81653935185</v>
+        <v>45947.860578703701</v>
       </c>
       <c r="B34">
         <v>9</v>
@@ -2378,7 +2348,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>45946.81653935185</v>
+        <v>45947.860578703701</v>
       </c>
       <c r="B35">
         <v>9</v>
@@ -2419,7 +2389,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>45946.81653935185</v>
+        <v>45947.860578703701</v>
       </c>
       <c r="B36">
         <v>9</v>
@@ -2460,7 +2430,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>45946.81653935185</v>
+        <v>45947.860578703701</v>
       </c>
       <c r="B37">
         <v>9</v>
@@ -2469,13 +2439,13 @@
         <v>16</v>
       </c>
       <c r="D37">
-        <v>10745.9012</v>
+        <v>10745.928599999999</v>
       </c>
       <c r="E37">
         <v>0.875</v>
       </c>
       <c r="F37">
-        <v>1128.0005000000001</v>
+        <v>1127.9947999999999</v>
       </c>
       <c r="G37">
         <v>5000</v>
@@ -2487,21 +2457,21 @@
         <v>0</v>
       </c>
       <c r="J37">
-        <v>41.285844060000002</v>
+        <v>41.285834620000003</v>
       </c>
       <c r="K37">
-        <v>-2206.4357928200002</v>
+        <v>-2206.4442810999999</v>
       </c>
       <c r="L37">
-        <v>-18512.038290619999</v>
+        <v>-18512.029802339999</v>
       </c>
       <c r="M37">
-        <v>-20718.47408344</v>
+        <v>-20718.474083429999</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>45946.816550925927</v>
+        <v>45947.860659722224</v>
       </c>
       <c r="B38">
         <v>10</v>
@@ -2542,7 +2512,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>45946.816550925927</v>
+        <v>45947.860659722224</v>
       </c>
       <c r="B39">
         <v>10</v>
@@ -2583,7 +2553,7 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>45946.816550925927</v>
+        <v>45947.860659722224</v>
       </c>
       <c r="B40">
         <v>10</v>
@@ -2624,7 +2594,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>45946.816550925927</v>
+        <v>45947.860659722224</v>
       </c>
       <c r="B41">
         <v>10</v>
@@ -2633,13 +2603,13 @@
         <v>16</v>
       </c>
       <c r="D41">
-        <v>22067.8315</v>
+        <v>19592.829399999999</v>
       </c>
       <c r="E41">
-        <v>0.75</v>
+        <v>0.78120000000000001</v>
       </c>
       <c r="F41">
-        <v>220.99090000000001</v>
+        <v>438.8519</v>
       </c>
       <c r="G41">
         <v>5000</v>
@@ -2648,24 +2618,24 @@
         <v>25498.888470490001</v>
       </c>
       <c r="I41">
-        <v>9.9708031100000003</v>
+        <v>4.5193447899999999</v>
       </c>
       <c r="J41">
-        <v>40.125520520000002</v>
+        <v>40.755612139999997</v>
       </c>
       <c r="K41">
-        <v>-5678.4716004800002</v>
+        <v>-4932.9370101900004</v>
       </c>
       <c r="L41">
-        <v>-17164.058417370001</v>
+        <v>-17909.593007660002</v>
       </c>
       <c r="M41">
-        <v>-22842.53001785</v>
+        <v>-22842.530017839999</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>45946.816550925927</v>
+        <v>45947.860671296294</v>
       </c>
       <c r="B42">
         <v>11</v>
@@ -2706,7 +2676,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>45946.816550925927</v>
+        <v>45947.860671296294</v>
       </c>
       <c r="B43">
         <v>11</v>
@@ -2747,7 +2717,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>45946.816550925927</v>
+        <v>45947.860671296294</v>
       </c>
       <c r="B44">
         <v>11</v>
@@ -2788,7 +2758,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>45946.816550925927</v>
+        <v>45947.860671296294</v>
       </c>
       <c r="B45">
         <v>11</v>
@@ -2797,13 +2767,13 @@
         <v>16</v>
       </c>
       <c r="D45">
-        <v>21426.517500000002</v>
+        <v>23793.494299999998</v>
       </c>
       <c r="E45">
         <v>0.75</v>
       </c>
       <c r="F45">
-        <v>870.83630000000005</v>
+        <v>381.17840000000001</v>
       </c>
       <c r="G45">
         <v>5000</v>
@@ -2812,16 +2782,16 @@
         <v>19532.688727550001</v>
       </c>
       <c r="I45">
-        <v>16.143879139999999</v>
+        <v>17.461622120000001</v>
       </c>
       <c r="J45">
-        <v>41.769314199999997</v>
+        <v>41.330066539999997</v>
       </c>
       <c r="K45">
-        <v>-6538.8272827399996</v>
+        <v>-6720.7907467300001</v>
       </c>
       <c r="L45">
-        <v>-20232.117059259999</v>
+        <v>-20050.15359528</v>
       </c>
       <c r="M45">
         <v>-26770.94434201</v>
@@ -2829,7 +2799,7 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>45946.816574074073</v>
+        <v>45947.860682870371</v>
       </c>
       <c r="B46">
         <v>12</v>
@@ -2870,7 +2840,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>45946.816574074073</v>
+        <v>45947.860682870371</v>
       </c>
       <c r="B47">
         <v>12</v>
@@ -2911,7 +2881,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>45946.816574074073</v>
+        <v>45947.860682870371</v>
       </c>
       <c r="B48">
         <v>12</v>
@@ -2952,7 +2922,7 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>45946.816574074073</v>
+        <v>45947.860682870371</v>
       </c>
       <c r="B49">
         <v>12</v>
@@ -2961,13 +2931,13 @@
         <v>16</v>
       </c>
       <c r="D49">
-        <v>9924.5110000000004</v>
+        <v>9924.5170999999991</v>
       </c>
       <c r="E49">
         <v>0.875</v>
       </c>
       <c r="F49">
-        <v>232.20939999999999</v>
+        <v>232.2063</v>
       </c>
       <c r="G49">
         <v>5000</v>
@@ -2979,13 +2949,13 @@
         <v>0</v>
       </c>
       <c r="J49">
-        <v>32.75514029</v>
+        <v>32.755139990000004</v>
       </c>
       <c r="K49">
-        <v>-1933.2214097900001</v>
+        <v>-1933.2225555099999</v>
       </c>
       <c r="L49">
-        <v>-13552.924697660001</v>
+        <v>-13552.92355193</v>
       </c>
       <c r="M49">
         <v>-15486.146107439999</v>
@@ -2993,7 +2963,7 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>45946.81658564815</v>
+        <v>45947.860706018517</v>
       </c>
       <c r="B50">
         <v>13</v>
@@ -3034,7 +3004,7 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>45946.81658564815</v>
+        <v>45947.860706018517</v>
       </c>
       <c r="B51">
         <v>13</v>
@@ -3075,7 +3045,7 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>45946.81658564815</v>
+        <v>45947.860706018517</v>
       </c>
       <c r="B52">
         <v>13</v>
@@ -3116,7 +3086,7 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>45946.81658564815</v>
+        <v>45947.860706018517</v>
       </c>
       <c r="B53">
         <v>13</v>
@@ -3125,13 +3095,13 @@
         <v>16</v>
       </c>
       <c r="D53">
-        <v>10634.760200000001</v>
+        <v>10634.7469</v>
       </c>
       <c r="E53">
         <v>0.875</v>
       </c>
       <c r="F53">
-        <v>484.93610000000001</v>
+        <v>484.9402</v>
       </c>
       <c r="G53">
         <v>5000</v>
@@ -3143,13 +3113,13 @@
         <v>0</v>
       </c>
       <c r="J53">
-        <v>34.015187419999997</v>
+        <v>34.015192980000002</v>
       </c>
       <c r="K53">
-        <v>-2108.42341592</v>
+        <v>-2108.4189902600001</v>
       </c>
       <c r="L53">
-        <v>-15272.71284097</v>
+        <v>-15272.71726662</v>
       </c>
       <c r="M53">
         <v>-17381.13625688</v>
@@ -3157,7 +3127,7 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>45946.816608796296</v>
+        <v>45947.860729166663</v>
       </c>
       <c r="B54">
         <v>14</v>
@@ -3198,7 +3168,7 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>45946.816608796296</v>
+        <v>45947.860729166663</v>
       </c>
       <c r="B55">
         <v>14</v>
@@ -3239,7 +3209,7 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>45946.816608796296</v>
+        <v>45947.860729166663</v>
       </c>
       <c r="B56">
         <v>14</v>
@@ -3280,7 +3250,7 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>45946.816608796296</v>
+        <v>45947.860729166663</v>
       </c>
       <c r="B57">
         <v>14</v>
@@ -3289,13 +3259,13 @@
         <v>16</v>
       </c>
       <c r="D57">
-        <v>20646.2598</v>
+        <v>20646.260699999999</v>
       </c>
       <c r="E57">
         <v>0.75</v>
       </c>
       <c r="F57">
-        <v>197.1773</v>
+        <v>197.1772</v>
       </c>
       <c r="G57">
         <v>5000</v>
@@ -3304,16 +3274,16 @@
         <v>28711.233572900001</v>
       </c>
       <c r="I57">
-        <v>5.06451165</v>
+        <v>5.0645137499999997</v>
       </c>
       <c r="J57">
-        <v>43.384232599999997</v>
+        <v>43.384232220000001</v>
       </c>
       <c r="K57">
-        <v>-5007.8491251799996</v>
+        <v>-5007.8493796700004</v>
       </c>
       <c r="L57">
-        <v>-15861.07736617</v>
+        <v>-15861.07711169</v>
       </c>
       <c r="M57">
         <v>-20868.926491350001</v>
@@ -3321,7 +3291,7 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>45946.816620370373</v>
+        <v>45947.860763888886</v>
       </c>
       <c r="B58">
         <v>15</v>
@@ -3362,7 +3332,7 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>45946.816620370373</v>
+        <v>45947.860763888886</v>
       </c>
       <c r="B59">
         <v>15</v>
@@ -3403,7 +3373,7 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>45946.816620370373</v>
+        <v>45947.860763888886</v>
       </c>
       <c r="B60">
         <v>15</v>
@@ -3444,7 +3414,7 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>45946.816620370373</v>
+        <v>45947.860763888886</v>
       </c>
       <c r="B61">
         <v>15</v>
@@ -3453,13 +3423,13 @@
         <v>16</v>
       </c>
       <c r="D61">
-        <v>34826.899400000002</v>
+        <v>26364.216</v>
       </c>
       <c r="E61">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
       <c r="F61">
-        <v>734.49969999999996</v>
+        <v>1985.6719000000001</v>
       </c>
       <c r="G61">
         <v>5000</v>
@@ -3468,16 +3438,16 @@
         <v>13440.173378830001</v>
       </c>
       <c r="I61">
-        <v>29.910097199999999</v>
+        <v>14.57321394</v>
       </c>
       <c r="J61">
-        <v>49.279679430000002</v>
+        <v>53.94685501</v>
       </c>
       <c r="K61">
-        <v>-7284.0751644000002</v>
+        <v>-5912.1127789299999</v>
       </c>
       <c r="L61">
-        <v>-11677.81662603</v>
+        <v>-13049.779011500001</v>
       </c>
       <c r="M61">
         <v>-18961.89179043</v>
@@ -3485,7 +3455,7 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>45946.816712962966</v>
+        <v>45947.860856481479</v>
       </c>
       <c r="B62">
         <v>16</v>
@@ -3526,7 +3496,7 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>45946.816712962966</v>
+        <v>45947.860856481479</v>
       </c>
       <c r="B63">
         <v>16</v>
@@ -3567,7 +3537,7 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>45946.816712962966</v>
+        <v>45947.860856481479</v>
       </c>
       <c r="B64">
         <v>16</v>
@@ -3608,7 +3578,7 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>45946.816712962966</v>
+        <v>45947.860856481479</v>
       </c>
       <c r="B65">
         <v>16</v>
@@ -3617,13 +3587,13 @@
         <v>16</v>
       </c>
       <c r="D65">
-        <v>76301.616500000004</v>
+        <v>76404.731199999995</v>
       </c>
       <c r="E65">
-        <v>0.17069999999999999</v>
+        <v>0.16739999999999999</v>
       </c>
       <c r="F65">
-        <v>482.47379999999998</v>
+        <v>480.70479999999998</v>
       </c>
       <c r="G65">
         <v>5000</v>
@@ -3632,24 +3602,24 @@
         <v>2158.9006670899998</v>
       </c>
       <c r="I65">
-        <v>56.40478684</v>
+        <v>56.413239750000002</v>
       </c>
       <c r="J65">
         <v>0</v>
       </c>
       <c r="K65">
-        <v>-9709.9596186599993</v>
+        <v>-9710.2480072899998</v>
       </c>
       <c r="L65">
-        <v>-2175.0516117000002</v>
+        <v>-2174.9931571400002</v>
       </c>
       <c r="M65">
-        <v>-11885.01123036</v>
+        <v>-11885.241164429999</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>45946.816747685189</v>
+        <v>45947.860891203702</v>
       </c>
       <c r="B66">
         <v>17</v>
@@ -3690,7 +3660,7 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>45946.816747685189</v>
+        <v>45947.860891203702</v>
       </c>
       <c r="B67">
         <v>17</v>
@@ -3731,7 +3701,7 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>45946.816747685189</v>
+        <v>45947.860891203702</v>
       </c>
       <c r="B68">
         <v>17</v>
@@ -3772,7 +3742,7 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>45946.816747685189</v>
+        <v>45947.860891203702</v>
       </c>
       <c r="B69">
         <v>17</v>
@@ -3781,13 +3751,13 @@
         <v>16</v>
       </c>
       <c r="D69">
-        <v>8287.1337999999996</v>
+        <v>7146.3074999999999</v>
       </c>
       <c r="E69">
-        <v>0.90620000000000001</v>
+        <v>0.9375</v>
       </c>
       <c r="F69">
-        <v>103.78919999999999</v>
+        <v>168.30350000000001</v>
       </c>
       <c r="G69">
         <v>5000</v>
@@ -3799,13 +3769,13 @@
         <v>0</v>
       </c>
       <c r="J69">
-        <v>34.596862090000002</v>
+        <v>35.140050770000002</v>
       </c>
       <c r="K69">
-        <v>-1570.1525390700001</v>
+        <v>-1039.98274214</v>
       </c>
       <c r="L69">
-        <v>-15253.96443876</v>
+        <v>-15784.13423569</v>
       </c>
       <c r="M69">
         <v>-16824.116977819998</v>
@@ -3813,7 +3783,7 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>45946.816759259258</v>
+        <v>45947.860914351855</v>
       </c>
       <c r="B70">
         <v>18</v>
@@ -3854,7 +3824,7 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>45946.816759259258</v>
+        <v>45947.860914351855</v>
       </c>
       <c r="B71">
         <v>18</v>
@@ -3895,7 +3865,7 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>45946.816759259258</v>
+        <v>45947.860914351855</v>
       </c>
       <c r="B72">
         <v>18</v>
@@ -3936,7 +3906,7 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>45946.816759259258</v>
+        <v>45947.860914351855</v>
       </c>
       <c r="B73">
         <v>18</v>
@@ -3945,13 +3915,13 @@
         <v>16</v>
       </c>
       <c r="D73">
-        <v>7248.4790000000003</v>
+        <v>10317.062599999999</v>
       </c>
       <c r="E73">
-        <v>0.9375</v>
+        <v>0.875</v>
       </c>
       <c r="F73">
-        <v>464.8177</v>
+        <v>179.19829999999999</v>
       </c>
       <c r="G73">
         <v>5000</v>
@@ -3963,13 +3933,13 @@
         <v>0</v>
       </c>
       <c r="J73">
-        <v>35.537950819999999</v>
+        <v>34.250918579999997</v>
       </c>
       <c r="K73">
-        <v>-1019.3310087</v>
+        <v>-2201.3104826899998</v>
       </c>
       <c r="L73">
-        <v>-16901.885641929999</v>
+        <v>-15719.906167929999</v>
       </c>
       <c r="M73">
         <v>-17921.216650620001</v>
@@ -3977,7 +3947,7 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>45946.816782407404</v>
+        <v>45947.860925925925</v>
       </c>
       <c r="B74">
         <v>19</v>
@@ -4018,7 +3988,7 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>45946.816782407404</v>
+        <v>45947.860925925925</v>
       </c>
       <c r="B75">
         <v>19</v>
@@ -4059,7 +4029,7 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>45946.816782407404</v>
+        <v>45947.860925925925</v>
       </c>
       <c r="B76">
         <v>19</v>
@@ -4100,7 +4070,7 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>45946.816782407404</v>
+        <v>45947.860925925925</v>
       </c>
       <c r="B77">
         <v>19</v>
@@ -4109,13 +4079,13 @@
         <v>16</v>
       </c>
       <c r="D77">
-        <v>20157.3436</v>
+        <v>20157.359100000001</v>
       </c>
       <c r="E77">
         <v>0.75</v>
       </c>
       <c r="F77">
-        <v>529.45619999999997</v>
+        <v>529.45280000000002</v>
       </c>
       <c r="G77">
         <v>5000</v>
@@ -4124,16 +4094,16 @@
         <v>27546.249180729999</v>
       </c>
       <c r="I77">
-        <v>2.2254577200000001</v>
+        <v>2.2254817500000001</v>
       </c>
       <c r="J77">
-        <v>42.546656059999997</v>
+        <v>42.54664957</v>
       </c>
       <c r="K77">
-        <v>-4612.8385285300001</v>
+        <v>-4612.8425213700002</v>
       </c>
       <c r="L77">
-        <v>-15178.89435633</v>
+        <v>-15178.89036349</v>
       </c>
       <c r="M77">
         <v>-19791.732884860001</v>
@@ -4141,7 +4111,7 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>45946.816805555558</v>
+        <v>45947.860949074071</v>
       </c>
       <c r="B78">
         <v>20</v>
@@ -4182,7 +4152,7 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>45946.816805555558</v>
+        <v>45947.860949074071</v>
       </c>
       <c r="B79">
         <v>20</v>
@@ -4223,7 +4193,7 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>45946.816805555558</v>
+        <v>45947.860949074071</v>
       </c>
       <c r="B80">
         <v>20</v>
@@ -4264,7 +4234,7 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>45946.816805555558</v>
+        <v>45947.860949074071</v>
       </c>
       <c r="B81">
         <v>20</v>
@@ -4273,13 +4243,13 @@
         <v>16</v>
       </c>
       <c r="D81">
-        <v>29436.2052</v>
+        <v>29437.116099999999</v>
       </c>
       <c r="E81">
         <v>0.5625</v>
       </c>
       <c r="F81">
-        <v>2288.1288</v>
+        <v>2287.8975999999998</v>
       </c>
       <c r="G81">
         <v>5000</v>
@@ -4288,16 +4258,16 @@
         <v>14617.29105048</v>
       </c>
       <c r="I81">
-        <v>16.1363071</v>
+        <v>16.13772861</v>
       </c>
       <c r="J81">
-        <v>45.241892630000002</v>
+        <v>45.241504140000004</v>
       </c>
       <c r="K81">
-        <v>-5961.7117948900004</v>
+        <v>-5961.8324848900002</v>
       </c>
       <c r="L81">
-        <v>-11599.620569799999</v>
+        <v>-11599.4998798</v>
       </c>
       <c r="M81">
         <v>-17561.332364689999</v>
@@ -4305,7 +4275,7 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>45946.81690972222</v>
+        <v>45947.861041666663</v>
       </c>
       <c r="B82">
         <v>21</v>
@@ -4346,7 +4316,7 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>45946.81690972222</v>
+        <v>45947.861041666663</v>
       </c>
       <c r="B83">
         <v>21</v>
@@ -4387,7 +4357,7 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>45946.81690972222</v>
+        <v>45947.861041666663</v>
       </c>
       <c r="B84">
         <v>21</v>
@@ -4428,7 +4398,7 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>45946.81690972222</v>
+        <v>45947.861041666663</v>
       </c>
       <c r="B85">
         <v>21</v>
@@ -4437,13 +4407,13 @@
         <v>16</v>
       </c>
       <c r="D85">
-        <v>42088.082799999996</v>
+        <v>42235.6584</v>
       </c>
       <c r="E85">
-        <v>0.3044</v>
+        <v>0.3009</v>
       </c>
       <c r="F85">
-        <v>7965.2385000000004</v>
+        <v>7947.3869000000004</v>
       </c>
       <c r="G85">
         <v>5000</v>
@@ -4452,24 +4422,24 @@
         <v>4398.4306578300002</v>
       </c>
       <c r="I85">
-        <v>32.346891370000002</v>
+        <v>32.37888985</v>
       </c>
       <c r="J85">
-        <v>-78.175985280000006</v>
+        <v>-80.015788369999996</v>
       </c>
       <c r="K85">
-        <v>-7698.2122110999999</v>
+        <v>-7700.7848825000001</v>
       </c>
       <c r="L85">
-        <v>-4836.6033193100002</v>
+        <v>-4835.6387412499998</v>
       </c>
       <c r="M85">
-        <v>-12534.81553041</v>
+        <v>-12536.423623750001</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>45946.817094907405</v>
+        <v>45947.861238425925</v>
       </c>
       <c r="B86">
         <v>22</v>
@@ -4510,7 +4480,7 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>45946.817094907405</v>
+        <v>45947.861238425925</v>
       </c>
       <c r="B87">
         <v>22</v>
@@ -4551,7 +4521,7 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>45946.817094907405</v>
+        <v>45947.861238425925</v>
       </c>
       <c r="B88">
         <v>22</v>
@@ -4592,7 +4562,7 @@
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>45946.817094907405</v>
+        <v>45947.861238425925</v>
       </c>
       <c r="B89">
         <v>22</v>
@@ -4633,7 +4603,7 @@
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>45946.817106481481</v>
+        <v>45947.861261574071</v>
       </c>
       <c r="B90">
         <v>23</v>
@@ -4674,7 +4644,7 @@
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>45946.817106481481</v>
+        <v>45947.861261574071</v>
       </c>
       <c r="B91">
         <v>23</v>
@@ -4715,7 +4685,7 @@
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>45946.817106481481</v>
+        <v>45947.861261574071</v>
       </c>
       <c r="B92">
         <v>23</v>
@@ -4756,7 +4726,7 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>45946.817106481481</v>
+        <v>45947.861261574071</v>
       </c>
       <c r="B93">
         <v>23</v>
@@ -4765,13 +4735,13 @@
         <v>16</v>
       </c>
       <c r="D93">
-        <v>15927.848</v>
+        <v>11935.588299999999</v>
       </c>
       <c r="E93">
-        <v>0.75</v>
+        <v>0.8125</v>
       </c>
       <c r="F93">
-        <v>456.81990000000002</v>
+        <v>953.00099999999998</v>
       </c>
       <c r="G93">
         <v>5000</v>
@@ -4783,13 +4753,13 @@
         <v>0</v>
       </c>
       <c r="J93">
-        <v>31.61902035</v>
+        <v>34.201445380000003</v>
       </c>
       <c r="K93">
-        <v>-3602.83013673</v>
+        <v>-2464.9819020599998</v>
       </c>
       <c r="L93">
-        <v>-11518.37797981</v>
+        <v>-12656.226214480001</v>
       </c>
       <c r="M93">
         <v>-15121.20811654</v>
@@ -4797,7 +4767,7 @@
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>45946.817118055558</v>
+        <v>45947.861273148148</v>
       </c>
       <c r="B94">
         <v>24</v>
@@ -4838,7 +4808,7 @@
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>45946.817118055558</v>
+        <v>45947.861273148148</v>
       </c>
       <c r="B95">
         <v>24</v>
@@ -4879,7 +4849,7 @@
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>45946.817118055558</v>
+        <v>45947.861273148148</v>
       </c>
       <c r="B96">
         <v>24</v>
@@ -4920,7 +4890,7 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>45946.817118055558</v>
+        <v>45947.861273148148</v>
       </c>
       <c r="B97">
         <v>24</v>
@@ -4929,13 +4899,13 @@
         <v>16</v>
       </c>
       <c r="D97">
-        <v>14486.4031</v>
+        <v>14486.3529</v>
       </c>
       <c r="E97">
         <v>0.875</v>
       </c>
       <c r="F97">
-        <v>95.612499999999997</v>
+        <v>95.622900000000001</v>
       </c>
       <c r="G97">
         <v>5000</v>
@@ -4947,13 +4917,13 @@
         <v>0</v>
       </c>
       <c r="J97">
-        <v>45.662572670000003</v>
+        <v>45.662582700000002</v>
       </c>
       <c r="K97">
-        <v>-3588.9577042699998</v>
+        <v>-3588.9398206400001</v>
       </c>
       <c r="L97">
-        <v>-25541.294735399999</v>
+        <v>-25541.312619029999</v>
       </c>
       <c r="M97">
         <v>-29130.252439669999</v>
@@ -4961,7 +4931,7 @@
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>45946.817141203705</v>
+        <v>45947.861296296294</v>
       </c>
       <c r="B98">
         <v>25</v>
@@ -5002,7 +4972,7 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>45946.817141203705</v>
+        <v>45947.861296296294</v>
       </c>
       <c r="B99">
         <v>25</v>
@@ -5043,7 +5013,7 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>45946.817141203705</v>
+        <v>45947.861296296294</v>
       </c>
       <c r="B100">
         <v>25</v>
@@ -5084,7 +5054,7 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>45946.817141203705</v>
+        <v>45947.861296296294</v>
       </c>
       <c r="B101">
         <v>25</v>
@@ -5093,13 +5063,13 @@
         <v>16</v>
       </c>
       <c r="D101">
-        <v>8738.4058999999997</v>
+        <v>8738.3091000000004</v>
       </c>
       <c r="E101">
         <v>0.9375</v>
       </c>
       <c r="F101">
-        <v>955.00400000000002</v>
+        <v>955.024</v>
       </c>
       <c r="G101">
         <v>5000</v>
@@ -5111,16 +5081,180 @@
         <v>0</v>
       </c>
       <c r="J101">
-        <v>48.580336379999999</v>
+        <v>48.580346239999997</v>
       </c>
       <c r="K101">
-        <v>-1882.68350601</v>
+        <v>-1882.6483449499999</v>
       </c>
       <c r="L101">
-        <v>-37196.219474609999</v>
+        <v>-37196.25463566</v>
       </c>
       <c r="M101">
         <v>-39078.902980610001</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>45947.861307870371</v>
+      </c>
+      <c r="B102">
+        <v>26</v>
+      </c>
+      <c r="C102" t="s">
+        <v>13</v>
+      </c>
+      <c r="D102">
+        <v>37261.088199999998</v>
+      </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+      <c r="G102">
+        <v>5000</v>
+      </c>
+      <c r="H102">
+        <v>126924.28410044999</v>
+      </c>
+      <c r="I102">
+        <v>30.001638710000002</v>
+      </c>
+      <c r="J102">
+        <v>49.259398019999999</v>
+      </c>
+      <c r="K102">
+        <v>-10440.156118250001</v>
+      </c>
+      <c r="L102">
+        <v>-45059.767213719999</v>
+      </c>
+      <c r="M102">
+        <v>-55499.92333197</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>45947.861307870371</v>
+      </c>
+      <c r="B103">
+        <v>26</v>
+      </c>
+      <c r="C103" t="s">
+        <v>14</v>
+      </c>
+      <c r="D103">
+        <v>13623.438200000001</v>
+      </c>
+      <c r="E103">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="F103">
+        <v>0</v>
+      </c>
+      <c r="G103">
+        <v>5000</v>
+      </c>
+      <c r="H103">
+        <v>126924.28410044999</v>
+      </c>
+      <c r="I103">
+        <v>0</v>
+      </c>
+      <c r="J103">
+        <v>49.393381939999998</v>
+      </c>
+      <c r="K103">
+        <v>-3596.6489545999998</v>
+      </c>
+      <c r="L103">
+        <v>-45650.201251309998</v>
+      </c>
+      <c r="M103">
+        <v>-49246.850205909999</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>45947.861307870371</v>
+      </c>
+      <c r="B104">
+        <v>26</v>
+      </c>
+      <c r="C104" t="s">
+        <v>15</v>
+      </c>
+      <c r="D104">
+        <v>37261.088199999998</v>
+      </c>
+      <c r="E104">
+        <v>0</v>
+      </c>
+      <c r="F104">
+        <v>0</v>
+      </c>
+      <c r="G104">
+        <v>5000</v>
+      </c>
+      <c r="H104">
+        <v>126924.28410044999</v>
+      </c>
+      <c r="I104">
+        <v>30.001638710000002</v>
+      </c>
+      <c r="J104">
+        <v>49.259398019999999</v>
+      </c>
+      <c r="K104">
+        <v>-10440.156118250001</v>
+      </c>
+      <c r="L104">
+        <v>-45059.767213719999</v>
+      </c>
+      <c r="M104">
+        <v>-55499.92333197</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>45947.861307870371</v>
+      </c>
+      <c r="B105">
+        <v>26</v>
+      </c>
+      <c r="C105" t="s">
+        <v>16</v>
+      </c>
+      <c r="D105">
+        <v>11298.3189</v>
+      </c>
+      <c r="E105">
+        <v>0.9375</v>
+      </c>
+      <c r="F105">
+        <v>425.43329999999997</v>
+      </c>
+      <c r="G105">
+        <v>5000</v>
+      </c>
+      <c r="H105">
+        <v>126924.28410044999</v>
+      </c>
+      <c r="I105">
+        <v>0</v>
+      </c>
+      <c r="J105">
+        <v>49.548608289999997</v>
+      </c>
+      <c r="K105">
+        <v>-2818.0748258200001</v>
+      </c>
+      <c r="L105">
+        <v>-46428.775380090003</v>
+      </c>
+      <c r="M105">
+        <v>-49246.850205909999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>